<commit_message>
Add in TSTool command file to process data from xlsx to geojson and add in geojson file; update README
</commit_message>
<xml_diff>
--- a/data/Colorado-Municipalities.xlsx
+++ b/data/Colorado-Municipalities.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="3" r:id="rId1"/>
@@ -53,7 +53,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>owf:</t>
         </r>
@@ -62,7 +62,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 5-digit Federal Information Processing Standard ID</t>
@@ -161,7 +161,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>owf:</t>
         </r>
@@ -170,7 +170,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 5-digit Colorado Department of Local Affairs' Local Government ID</t>
@@ -2998,50 +2998,6 @@
     <t>x</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Latitude</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Longitude</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> coordinates were found by accessing a Colorado Information Marketplace map titled "Municipal Boundaries in Colorado" (https://data.colorado.gov/Municipal/Municipal-Boundaries-in-Colorado/u943-ics6).  The map was downloaded as a GeoJSON file and opened in QGIS.  The centroid of each municipality's polygon was calculated and used as the point location for the municipality.  The original GeoJSON file can be found at:  data-orig/Colorado-Municipal-Boundaries.geojson.  The attribute table that was saved as a csv and contains coordinate data can be found at:  data-orig/Colorado-Municipalities-PointLocation.csv.</t>
-    </r>
-  </si>
-  <si>
     <t>Single-character indication of data status as it pertains to missing Water District IDs</t>
   </si>
   <si>
@@ -4549,6 +4505,50 @@
   <si>
     <t>66636</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Latitude</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Longitude</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> coordinates were found by accessing a Colorado Information Marketplace map titled "Municipal Boundaries in Colorado" (https://data.colorado.gov/Municipal/Municipal-Boundaries-in-Colorado/u943-ics6).  The map was downloaded as a GeoJSON file and opened in QGIS.  The centroid of each municipality's polygon was calculated and used as the point location for the municipality.  The attribute table that was saved as a csv and contains coordinate data can be found at:  data-orig/Colorado-Municipalities-PointLocation.csv.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -4558,7 +4558,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4607,19 +4607,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -4730,42 +4717,6 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -4821,6 +4772,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -4828,6 +4785,36 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5255,7 +5242,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:U1048576" totalsRowShown="0" headerRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:U1048576" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:U1048576">
     <filterColumn colId="0">
       <customFilters>
@@ -5264,23 +5251,23 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="21">
-    <tableColumn id="1" name="MunicipalityName" dataDxfId="15"/>
-    <tableColumn id="22" name="FIPS_ID" dataDxfId="4"/>
-    <tableColumn id="12" name="FIPS_ID_Flag" dataDxfId="14"/>
-    <tableColumn id="3" name="GNIS_ID" dataDxfId="13"/>
+    <tableColumn id="1" name="MunicipalityName" dataDxfId="12"/>
+    <tableColumn id="22" name="FIPS_ID" dataDxfId="11"/>
+    <tableColumn id="12" name="FIPS_ID_Flag" dataDxfId="10"/>
+    <tableColumn id="3" name="GNIS_ID" dataDxfId="9"/>
     <tableColumn id="13" name="GNIS_ID_Flag"/>
-    <tableColumn id="23" name="DOLA_LG_ID" dataDxfId="3"/>
+    <tableColumn id="23" name="DOLA_LG_ID" dataDxfId="8"/>
     <tableColumn id="14" name="DOLA_LG_ID_Flag"/>
-    <tableColumn id="5" name="BNDSS_ID" dataDxfId="12"/>
-    <tableColumn id="15" name="BNDSS_ID_Flag" dataDxfId="11"/>
+    <tableColumn id="5" name="BNDSS_ID" dataDxfId="7"/>
+    <tableColumn id="15" name="BNDSS_ID_Flag" dataDxfId="6"/>
     <tableColumn id="6" name="PWS_ID"/>
-    <tableColumn id="16" name="PWS_ID_Flag" dataDxfId="10"/>
-    <tableColumn id="20" name="DWR_WaterDistrict_ID" dataDxfId="9"/>
-    <tableColumn id="21" name="DWR_WaterDistrict_ID_Flag" dataDxfId="8"/>
-    <tableColumn id="7" name="County_CSV" dataDxfId="7"/>
-    <tableColumn id="18" name="NumCounty" dataDxfId="6"/>
+    <tableColumn id="16" name="PWS_ID_Flag" dataDxfId="5"/>
+    <tableColumn id="20" name="DWR_WaterDistrict_ID" dataDxfId="4"/>
+    <tableColumn id="21" name="DWR_WaterDistrict_ID_Flag" dataDxfId="3"/>
+    <tableColumn id="7" name="County_CSV" dataDxfId="2"/>
+    <tableColumn id="18" name="NumCounty" dataDxfId="1"/>
     <tableColumn id="8" name="IBCC_Basin_CSV"/>
-    <tableColumn id="19" name="Num_IBCC_Basin" dataDxfId="5"/>
+    <tableColumn id="19" name="Num_IBCC_Basin" dataDxfId="0"/>
     <tableColumn id="9" name="Latitude"/>
     <tableColumn id="10" name="Longitude"/>
     <tableColumn id="17" name="Lat_Long_Flag"/>
@@ -5555,8 +5542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5572,7 +5559,7 @@
     </row>
     <row r="2" spans="1:17" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -5738,9 +5725,9 @@
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
     </row>
-    <row r="12" spans="1:17" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>793</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5775,7 +5762,7 @@
     </row>
     <row r="22" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="23" spans="1:1" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5812,11 +5799,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U517"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="L11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -5890,10 +5877,10 @@
         <v>747</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>685</v>
@@ -5925,7 +5912,7 @@
         <v>711</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>711</v>
@@ -5979,7 +5966,7 @@
         <v>711</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>711</v>
@@ -6087,7 +6074,7 @@
         <v>711</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>711</v>
@@ -6141,7 +6128,7 @@
         <v>711</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>711</v>
@@ -6195,7 +6182,7 @@
         <v>711</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>711</v>
@@ -6249,7 +6236,7 @@
         <v>711</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>711</v>
@@ -6303,7 +6290,7 @@
         <v>711</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>711</v>
@@ -6357,7 +6344,7 @@
         <v>711</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>711</v>
@@ -6414,7 +6401,7 @@
         <v>711</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>711</v>
@@ -6468,7 +6455,7 @@
         <v>711</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>711</v>
@@ -6522,7 +6509,7 @@
         <v>711</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>711</v>
@@ -6576,7 +6563,7 @@
         <v>711</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>711</v>
@@ -6630,7 +6617,7 @@
         <v>711</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>711</v>
@@ -6684,7 +6671,7 @@
         <v>711</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>711</v>
@@ -6738,7 +6725,7 @@
         <v>711</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>711</v>
@@ -6792,7 +6779,7 @@
         <v>711</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>711</v>
@@ -6846,7 +6833,7 @@
         <v>711</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>711</v>
@@ -6903,7 +6890,7 @@
         <v>711</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>711</v>
@@ -6958,7 +6945,7 @@
         <v>711</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>711</v>
@@ -7015,7 +7002,7 @@
         <v>711</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>711</v>
@@ -7123,7 +7110,7 @@
         <v>711</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>711</v>
@@ -7178,7 +7165,7 @@
         <v>711</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>711</v>
@@ -7235,7 +7222,7 @@
         <v>711</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>711</v>
@@ -7289,7 +7276,7 @@
         <v>711</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>711</v>
@@ -7343,7 +7330,7 @@
         <v>711</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>711</v>
@@ -7397,7 +7384,7 @@
         <v>711</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>711</v>
@@ -7451,7 +7438,7 @@
         <v>711</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>711</v>
@@ -7493,7 +7480,7 @@
         <v>120</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>711</v>
@@ -7547,7 +7534,7 @@
         <v>124</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>711</v>
@@ -7559,7 +7546,7 @@
         <v>711</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>711</v>
@@ -7601,7 +7588,7 @@
         <v>126</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>711</v>
@@ -7613,7 +7600,7 @@
         <v>711</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>711</v>
@@ -7658,7 +7645,7 @@
         <v>129</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>711</v>
@@ -7712,7 +7699,7 @@
         <v>132</v>
       </c>
       <c r="B35" s="32" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>711</v>
@@ -7724,7 +7711,7 @@
         <v>711</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>711</v>
@@ -7773,7 +7760,7 @@
         <v>712</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>711</v>
@@ -7816,7 +7803,7 @@
         <v>135</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>711</v>
@@ -7828,7 +7815,7 @@
         <v>711</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>711</v>
@@ -7870,7 +7857,7 @@
         <v>677</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>711</v>
@@ -7882,7 +7869,7 @@
         <v>711</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>711</v>
@@ -7925,7 +7912,7 @@
         <v>139</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>711</v>
@@ -7937,7 +7924,7 @@
         <v>711</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>711</v>
@@ -7979,7 +7966,7 @@
         <v>142</v>
       </c>
       <c r="B40" s="32" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>711</v>
@@ -7991,7 +7978,7 @@
         <v>711</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>711</v>
@@ -8033,7 +8020,7 @@
         <v>146</v>
       </c>
       <c r="B41" s="32" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>711</v>
@@ -8088,7 +8075,7 @@
         <v>148</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>711</v>
@@ -8100,7 +8087,7 @@
         <v>711</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>711</v>
@@ -8142,7 +8129,7 @@
         <v>151</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>711</v>
@@ -8154,7 +8141,7 @@
         <v>711</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>711</v>
@@ -8196,7 +8183,7 @@
         <v>155</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>711</v>
@@ -8208,7 +8195,7 @@
         <v>711</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>711</v>
@@ -8250,7 +8237,7 @@
         <v>158</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>711</v>
@@ -8303,7 +8290,7 @@
         <v>159</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>711</v>
@@ -8360,7 +8347,7 @@
         <v>162</v>
       </c>
       <c r="B47" s="32" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>711</v>
@@ -8372,7 +8359,7 @@
         <v>711</v>
       </c>
       <c r="F47" s="17" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>711</v>
@@ -8417,7 +8404,7 @@
         <v>164</v>
       </c>
       <c r="B48" s="32" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>711</v>
@@ -8429,7 +8416,7 @@
         <v>711</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>711</v>
@@ -8474,7 +8461,7 @@
         <v>166</v>
       </c>
       <c r="B49" s="32" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>711</v>
@@ -8486,7 +8473,7 @@
         <v>711</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>711</v>
@@ -8528,7 +8515,7 @@
         <v>169</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>711</v>
@@ -8540,7 +8527,7 @@
         <v>711</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>711</v>
@@ -8582,7 +8569,7 @@
         <v>172</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>711</v>
@@ -8637,7 +8624,7 @@
         <v>173</v>
       </c>
       <c r="B52" s="32" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>711</v>
@@ -8692,7 +8679,7 @@
         <v>175</v>
       </c>
       <c r="B53" s="32" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>711</v>
@@ -8704,7 +8691,7 @@
         <v>711</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>711</v>
@@ -8746,7 +8733,7 @@
         <v>178</v>
       </c>
       <c r="B54" s="32" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>711</v>
@@ -8758,7 +8745,7 @@
         <v>711</v>
       </c>
       <c r="F54" s="17" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>711</v>
@@ -8800,7 +8787,7 @@
         <v>182</v>
       </c>
       <c r="B55" s="32" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>711</v>
@@ -8812,7 +8799,7 @@
         <v>711</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>711</v>
@@ -8854,7 +8841,7 @@
         <v>184</v>
       </c>
       <c r="B56" s="32" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>711</v>
@@ -8866,7 +8853,7 @@
         <v>711</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>711</v>
@@ -8908,7 +8895,7 @@
         <v>187</v>
       </c>
       <c r="B57" s="32" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>711</v>
@@ -8920,7 +8907,7 @@
         <v>711</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>711</v>
@@ -8962,7 +8949,7 @@
         <v>190</v>
       </c>
       <c r="B58" s="32" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>711</v>
@@ -8974,7 +8961,7 @@
         <v>711</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>711</v>
@@ -9014,7 +9001,7 @@
         <v>191</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>711</v>
@@ -9026,7 +9013,7 @@
         <v>711</v>
       </c>
       <c r="F59" s="17" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>711</v>
@@ -9068,7 +9055,7 @@
         <v>195</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>711</v>
@@ -9080,7 +9067,7 @@
         <v>711</v>
       </c>
       <c r="F60" s="17" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>711</v>
@@ -9125,7 +9112,7 @@
         <v>198</v>
       </c>
       <c r="B61" s="32" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>711</v>
@@ -9137,7 +9124,7 @@
         <v>711</v>
       </c>
       <c r="F61" s="17" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>711</v>
@@ -9179,7 +9166,7 @@
         <v>200</v>
       </c>
       <c r="B62" s="32" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>711</v>
@@ -9191,7 +9178,7 @@
         <v>711</v>
       </c>
       <c r="F62" s="17" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>711</v>
@@ -9233,7 +9220,7 @@
         <v>202</v>
       </c>
       <c r="B63" s="32" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>711</v>
@@ -9245,7 +9232,7 @@
         <v>711</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>711</v>
@@ -9290,7 +9277,7 @@
         <v>204</v>
       </c>
       <c r="B64" s="32" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>711</v>
@@ -9347,7 +9334,7 @@
         <v>206</v>
       </c>
       <c r="B65" s="32" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>711</v>
@@ -9359,7 +9346,7 @@
         <v>711</v>
       </c>
       <c r="F65" s="17" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>711</v>
@@ -9401,7 +9388,7 @@
         <v>144</v>
       </c>
       <c r="B66" s="32" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>711</v>
@@ -9413,7 +9400,7 @@
         <v>711</v>
       </c>
       <c r="F66" s="17" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>711</v>
@@ -9455,7 +9442,7 @@
         <v>210</v>
       </c>
       <c r="B67" s="32" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>711</v>
@@ -9467,7 +9454,7 @@
         <v>711</v>
       </c>
       <c r="F67" s="17" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>711</v>
@@ -9509,7 +9496,7 @@
         <v>213</v>
       </c>
       <c r="B68" s="32" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>711</v>
@@ -9521,7 +9508,7 @@
         <v>711</v>
       </c>
       <c r="F68" s="17" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>711</v>
@@ -9563,7 +9550,7 @@
         <v>215</v>
       </c>
       <c r="B69" s="32" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>711</v>
@@ -9575,7 +9562,7 @@
         <v>711</v>
       </c>
       <c r="F69" s="17" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>711</v>
@@ -9617,7 +9604,7 @@
         <v>217</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>711</v>
@@ -9629,7 +9616,7 @@
         <v>711</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>711</v>
@@ -9671,7 +9658,7 @@
         <v>219</v>
       </c>
       <c r="B71" s="32" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>711</v>
@@ -9683,7 +9670,7 @@
         <v>711</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>711</v>
@@ -9728,7 +9715,7 @@
         <v>221</v>
       </c>
       <c r="B72" s="32" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>711</v>
@@ -9740,7 +9727,7 @@
         <v>711</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>711</v>
@@ -9782,7 +9769,7 @@
         <v>223</v>
       </c>
       <c r="B73" s="32" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>711</v>
@@ -9794,7 +9781,7 @@
         <v>711</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>711</v>
@@ -9836,7 +9823,7 @@
         <v>52</v>
       </c>
       <c r="B74" s="32" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>711</v>
@@ -9848,7 +9835,7 @@
         <v>711</v>
       </c>
       <c r="F74" s="17" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>711</v>
@@ -9890,7 +9877,7 @@
         <v>227</v>
       </c>
       <c r="B75" s="32" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>711</v>
@@ -9902,7 +9889,7 @@
         <v>711</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>711</v>
@@ -9944,7 +9931,7 @@
         <v>229</v>
       </c>
       <c r="B76" s="32" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>711</v>
@@ -9956,7 +9943,7 @@
         <v>711</v>
       </c>
       <c r="F76" s="17" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>711</v>
@@ -9998,7 +9985,7 @@
         <v>232</v>
       </c>
       <c r="B77" s="32" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>711</v>
@@ -10010,7 +9997,7 @@
         <v>711</v>
       </c>
       <c r="F77" s="17" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>711</v>
@@ -10052,7 +10039,7 @@
         <v>235</v>
       </c>
       <c r="B78" s="32" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>711</v>
@@ -10064,7 +10051,7 @@
         <v>711</v>
       </c>
       <c r="F78" s="17" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>711</v>
@@ -10109,7 +10096,7 @@
         <v>238</v>
       </c>
       <c r="B79" s="32" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>711</v>
@@ -10121,7 +10108,7 @@
         <v>711</v>
       </c>
       <c r="F79" s="17" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>711</v>
@@ -10163,7 +10150,7 @@
         <v>241</v>
       </c>
       <c r="B80" s="32" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>711</v>
@@ -10217,7 +10204,7 @@
         <v>243</v>
       </c>
       <c r="B81" s="32" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>711</v>
@@ -10229,7 +10216,7 @@
         <v>711</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>711</v>
@@ -10271,7 +10258,7 @@
         <v>246</v>
       </c>
       <c r="B82" s="32" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>711</v>
@@ -10283,7 +10270,7 @@
         <v>711</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>711</v>
@@ -10325,7 +10312,7 @@
         <v>250</v>
       </c>
       <c r="B83" s="32" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>711</v>
@@ -10337,7 +10324,7 @@
         <v>711</v>
       </c>
       <c r="F83" s="17" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>711</v>
@@ -10379,7 +10366,7 @@
         <v>252</v>
       </c>
       <c r="B84" s="32" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>711</v>
@@ -10391,7 +10378,7 @@
         <v>711</v>
       </c>
       <c r="F84" s="17" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>711</v>
@@ -10433,7 +10420,7 @@
         <v>254</v>
       </c>
       <c r="B85" s="32" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>711</v>
@@ -10488,7 +10475,7 @@
         <v>256</v>
       </c>
       <c r="B86" s="32" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>711</v>
@@ -10500,7 +10487,7 @@
         <v>711</v>
       </c>
       <c r="F86" s="17" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>711</v>
@@ -10542,7 +10529,7 @@
         <v>258</v>
       </c>
       <c r="B87" s="32" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>711</v>
@@ -10554,7 +10541,7 @@
         <v>711</v>
       </c>
       <c r="F87" s="17" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>711</v>
@@ -10596,7 +10583,7 @@
         <v>260</v>
       </c>
       <c r="B88" s="32" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>711</v>
@@ -10608,7 +10595,7 @@
         <v>711</v>
       </c>
       <c r="F88" s="17" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>711</v>
@@ -10653,7 +10640,7 @@
         <v>262</v>
       </c>
       <c r="B89" s="32" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>711</v>
@@ -10665,7 +10652,7 @@
         <v>711</v>
       </c>
       <c r="F89" s="17" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>711</v>
@@ -10707,7 +10694,7 @@
         <v>264</v>
       </c>
       <c r="B90" s="32" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>711</v>
@@ -10719,7 +10706,7 @@
         <v>711</v>
       </c>
       <c r="F90" s="17" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>711</v>
@@ -10762,7 +10749,7 @@
         <v>266</v>
       </c>
       <c r="B91" s="32" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>711</v>
@@ -10774,7 +10761,7 @@
         <v>711</v>
       </c>
       <c r="F91" s="17" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>711</v>
@@ -10816,7 +10803,7 @@
         <v>269</v>
       </c>
       <c r="B92" s="32" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>711</v>
@@ -10828,7 +10815,7 @@
         <v>711</v>
       </c>
       <c r="F92" s="17" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>711</v>
@@ -10870,7 +10857,7 @@
         <v>272</v>
       </c>
       <c r="B93" s="32" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>711</v>
@@ -10882,7 +10869,7 @@
         <v>711</v>
       </c>
       <c r="F93" s="17" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>711</v>
@@ -10924,7 +10911,7 @@
         <v>275</v>
       </c>
       <c r="B94" s="32" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>711</v>
@@ -10936,7 +10923,7 @@
         <v>711</v>
       </c>
       <c r="F94" s="17" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>711</v>
@@ -10978,7 +10965,7 @@
         <v>277</v>
       </c>
       <c r="B95" s="32" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>711</v>
@@ -11030,7 +11017,7 @@
         <v>278</v>
       </c>
       <c r="B96" s="32" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>711</v>
@@ -11042,7 +11029,7 @@
         <v>711</v>
       </c>
       <c r="F96" s="17" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>711</v>
@@ -11084,7 +11071,7 @@
         <v>281</v>
       </c>
       <c r="B97" s="32" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>711</v>
@@ -11096,7 +11083,7 @@
         <v>711</v>
       </c>
       <c r="F97" s="17" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>711</v>
@@ -11138,7 +11125,7 @@
         <v>283</v>
       </c>
       <c r="B98" s="32" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>711</v>
@@ -11150,7 +11137,7 @@
         <v>711</v>
       </c>
       <c r="F98" s="17" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>711</v>
@@ -11192,7 +11179,7 @@
         <v>285</v>
       </c>
       <c r="B99" s="32" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>711</v>
@@ -11204,7 +11191,7 @@
         <v>711</v>
       </c>
       <c r="F99" s="17" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>711</v>
@@ -11249,7 +11236,7 @@
         <v>287</v>
       </c>
       <c r="B100" s="32" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>711</v>
@@ -11261,7 +11248,7 @@
         <v>711</v>
       </c>
       <c r="F100" s="17" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>711</v>
@@ -11306,7 +11293,7 @@
         <v>289</v>
       </c>
       <c r="B101" s="32" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>711</v>
@@ -11318,7 +11305,7 @@
         <v>711</v>
       </c>
       <c r="F101" s="17" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>711</v>
@@ -11363,7 +11350,7 @@
         <v>291</v>
       </c>
       <c r="B102" s="32" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>711</v>
@@ -11375,7 +11362,7 @@
         <v>711</v>
       </c>
       <c r="F102" s="17" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>711</v>
@@ -11417,7 +11404,7 @@
         <v>293</v>
       </c>
       <c r="B103" s="32" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>711</v>
@@ -11429,7 +11416,7 @@
         <v>711</v>
       </c>
       <c r="F103" s="17" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>711</v>
@@ -11474,7 +11461,7 @@
         <v>295</v>
       </c>
       <c r="B104" s="32" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>711</v>
@@ -11528,7 +11515,7 @@
         <v>297</v>
       </c>
       <c r="B105" s="32" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>711</v>
@@ -11540,7 +11527,7 @@
         <v>711</v>
       </c>
       <c r="F105" s="17" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>711</v>
@@ -11582,7 +11569,7 @@
         <v>300</v>
       </c>
       <c r="B106" s="32" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>711</v>
@@ -11594,7 +11581,7 @@
         <v>711</v>
       </c>
       <c r="F106" s="17" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>711</v>
@@ -11636,7 +11623,7 @@
         <v>302</v>
       </c>
       <c r="B107" s="32" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>711</v>
@@ -11648,7 +11635,7 @@
         <v>711</v>
       </c>
       <c r="F107" s="17" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>711</v>
@@ -11693,7 +11680,7 @@
         <v>305</v>
       </c>
       <c r="B108" s="32" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>711</v>
@@ -11705,7 +11692,7 @@
         <v>711</v>
       </c>
       <c r="F108" s="17" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>711</v>
@@ -11747,7 +11734,7 @@
         <v>307</v>
       </c>
       <c r="B109" s="32" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>711</v>
@@ -11759,7 +11746,7 @@
         <v>711</v>
       </c>
       <c r="F109" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>711</v>
@@ -11801,7 +11788,7 @@
         <v>310</v>
       </c>
       <c r="B110" s="32" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>711</v>
@@ -11813,7 +11800,7 @@
         <v>711</v>
       </c>
       <c r="F110" s="17" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="G110" s="1" t="s">
         <v>711</v>
@@ -11855,7 +11842,7 @@
         <v>313</v>
       </c>
       <c r="B111" s="32" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>711</v>
@@ -11867,7 +11854,7 @@
         <v>711</v>
       </c>
       <c r="F111" s="17" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="G111" s="1" t="s">
         <v>711</v>
@@ -11909,7 +11896,7 @@
         <v>315</v>
       </c>
       <c r="B112" s="32" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>711</v>
@@ -11921,7 +11908,7 @@
         <v>711</v>
       </c>
       <c r="F112" s="17" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="G112" s="1" t="s">
         <v>711</v>
@@ -11963,7 +11950,7 @@
         <v>319</v>
       </c>
       <c r="B113" s="32" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>711</v>
@@ -12017,7 +12004,7 @@
         <v>322</v>
       </c>
       <c r="B114" s="32" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>711</v>
@@ -12029,7 +12016,7 @@
         <v>711</v>
       </c>
       <c r="F114" s="17" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="G114" s="1" t="s">
         <v>711</v>
@@ -12074,7 +12061,7 @@
         <v>145</v>
       </c>
       <c r="B115" s="32" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>711</v>
@@ -12086,7 +12073,7 @@
         <v>711</v>
       </c>
       <c r="F115" s="17" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>711</v>
@@ -12128,7 +12115,7 @@
         <v>325</v>
       </c>
       <c r="B116" s="32" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>711</v>
@@ -12140,7 +12127,7 @@
         <v>711</v>
       </c>
       <c r="F116" s="17" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="G116" s="1" t="s">
         <v>711</v>
@@ -12182,7 +12169,7 @@
         <v>327</v>
       </c>
       <c r="B117" s="32" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>711</v>
@@ -12194,7 +12181,7 @@
         <v>711</v>
       </c>
       <c r="F117" s="17" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="G117" s="1" t="s">
         <v>711</v>
@@ -12239,7 +12226,7 @@
         <v>329</v>
       </c>
       <c r="B118" s="32" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>711</v>
@@ -12251,7 +12238,7 @@
         <v>711</v>
       </c>
       <c r="F118" s="17" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="G118" s="1" t="s">
         <v>711</v>
@@ -12296,7 +12283,7 @@
         <v>331</v>
       </c>
       <c r="B119" s="32" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>711</v>
@@ -12308,7 +12295,7 @@
         <v>711</v>
       </c>
       <c r="F119" s="17" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="G119" s="1" t="s">
         <v>711</v>
@@ -12353,7 +12340,7 @@
         <v>334</v>
       </c>
       <c r="B120" s="32" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>711</v>
@@ -12365,7 +12352,7 @@
         <v>711</v>
       </c>
       <c r="F120" s="17" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="G120" s="1" t="s">
         <v>711</v>
@@ -12407,7 +12394,7 @@
         <v>337</v>
       </c>
       <c r="B121" s="32" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>711</v>
@@ -12419,7 +12406,7 @@
         <v>711</v>
       </c>
       <c r="F121" s="17" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="G121" s="1" t="s">
         <v>711</v>
@@ -12464,7 +12451,7 @@
         <v>339</v>
       </c>
       <c r="B122" s="32" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>711</v>
@@ -12476,7 +12463,7 @@
         <v>711</v>
       </c>
       <c r="F122" s="17" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="G122" s="1" t="s">
         <v>711</v>
@@ -12521,7 +12508,7 @@
         <v>341</v>
       </c>
       <c r="B123" s="32" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>711</v>
@@ -12533,7 +12520,7 @@
         <v>711</v>
       </c>
       <c r="F123" s="17" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>711</v>
@@ -12575,7 +12562,7 @@
         <v>343</v>
       </c>
       <c r="B124" s="32" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>711</v>
@@ -12630,7 +12617,7 @@
         <v>344</v>
       </c>
       <c r="B125" s="32" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>711</v>
@@ -12642,7 +12629,7 @@
         <v>711</v>
       </c>
       <c r="F125" s="17" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>711</v>
@@ -12684,7 +12671,7 @@
         <v>347</v>
       </c>
       <c r="B126" s="32" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>711</v>
@@ -12696,7 +12683,7 @@
         <v>711</v>
       </c>
       <c r="F126" s="17" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="G126" s="1" t="s">
         <v>711</v>
@@ -12738,7 +12725,7 @@
         <v>349</v>
       </c>
       <c r="B127" s="32" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>711</v>
@@ -12750,7 +12737,7 @@
         <v>711</v>
       </c>
       <c r="F127" s="17" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="G127" s="1" t="s">
         <v>711</v>
@@ -12792,7 +12779,7 @@
         <v>351</v>
       </c>
       <c r="B128" s="32" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>711</v>
@@ -12804,7 +12791,7 @@
         <v>711</v>
       </c>
       <c r="F128" s="17" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>711</v>
@@ -12846,7 +12833,7 @@
         <v>353</v>
       </c>
       <c r="B129" s="32" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>711</v>
@@ -12858,7 +12845,7 @@
         <v>711</v>
       </c>
       <c r="F129" s="17" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="G129" s="1" t="s">
         <v>711</v>
@@ -12900,7 +12887,7 @@
         <v>356</v>
       </c>
       <c r="B130" s="32" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>711</v>
@@ -12912,7 +12899,7 @@
         <v>711</v>
       </c>
       <c r="F130" s="17" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>711</v>
@@ -12954,7 +12941,7 @@
         <v>358</v>
       </c>
       <c r="B131" s="32" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>711</v>
@@ -12966,7 +12953,7 @@
         <v>711</v>
       </c>
       <c r="F131" s="17" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="G131" s="1" t="s">
         <v>711</v>
@@ -13011,7 +12998,7 @@
         <v>360</v>
       </c>
       <c r="B132" s="32" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>711</v>
@@ -13065,7 +13052,7 @@
         <v>362</v>
       </c>
       <c r="B133" s="32" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>711</v>
@@ -13077,7 +13064,7 @@
         <v>711</v>
       </c>
       <c r="F133" s="17" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="G133" s="1" t="s">
         <v>711</v>
@@ -13122,7 +13109,7 @@
         <v>364</v>
       </c>
       <c r="B134" s="32" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>711</v>
@@ -13134,7 +13121,7 @@
         <v>711</v>
       </c>
       <c r="F134" s="17" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="G134" s="1" t="s">
         <v>711</v>
@@ -13179,7 +13166,7 @@
         <v>367</v>
       </c>
       <c r="B135" s="32" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>711</v>
@@ -13191,7 +13178,7 @@
         <v>711</v>
       </c>
       <c r="F135" s="17" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="G135" s="1" t="s">
         <v>711</v>
@@ -13233,7 +13220,7 @@
         <v>369</v>
       </c>
       <c r="B136" s="32" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>711</v>
@@ -13245,7 +13232,7 @@
         <v>711</v>
       </c>
       <c r="F136" s="17" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="G136" s="1" t="s">
         <v>711</v>
@@ -13287,7 +13274,7 @@
         <v>371</v>
       </c>
       <c r="B137" s="32" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>711</v>
@@ -13299,7 +13286,7 @@
         <v>711</v>
       </c>
       <c r="F137" s="17" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G137" s="1" t="s">
         <v>711</v>
@@ -13344,7 +13331,7 @@
         <v>225</v>
       </c>
       <c r="B138" s="32" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>711</v>
@@ -13356,7 +13343,7 @@
         <v>711</v>
       </c>
       <c r="F138" s="17" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="G138" s="1" t="s">
         <v>711</v>
@@ -13398,7 +13385,7 @@
         <v>73</v>
       </c>
       <c r="B139" s="32" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>711</v>
@@ -13455,7 +13442,7 @@
         <v>375</v>
       </c>
       <c r="B140" s="32" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>711</v>
@@ -13467,7 +13454,7 @@
         <v>711</v>
       </c>
       <c r="F140" s="17" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="G140" s="1" t="s">
         <v>711</v>
@@ -13509,7 +13496,7 @@
         <v>377</v>
       </c>
       <c r="B141" s="32" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>711</v>
@@ -13521,7 +13508,7 @@
         <v>711</v>
       </c>
       <c r="F141" s="17" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="G141" s="1" t="s">
         <v>711</v>
@@ -13566,7 +13553,7 @@
         <v>379</v>
       </c>
       <c r="B142" s="32" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>711</v>
@@ -13578,7 +13565,7 @@
         <v>711</v>
       </c>
       <c r="F142" s="17" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="G142" s="1" t="s">
         <v>711</v>
@@ -13620,7 +13607,7 @@
         <v>382</v>
       </c>
       <c r="B143" s="32" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>711</v>
@@ -13632,7 +13619,7 @@
         <v>711</v>
       </c>
       <c r="F143" s="17" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="G143" s="1" t="s">
         <v>711</v>
@@ -13677,7 +13664,7 @@
         <v>384</v>
       </c>
       <c r="B144" s="32" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>711</v>
@@ -13689,7 +13676,7 @@
         <v>711</v>
       </c>
       <c r="F144" s="17" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="G144" s="1" t="s">
         <v>711</v>
@@ -13731,7 +13718,7 @@
         <v>388</v>
       </c>
       <c r="B145" s="32" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>711</v>
@@ -13785,7 +13772,7 @@
         <v>390</v>
       </c>
       <c r="B146" s="32" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>711</v>
@@ -13797,7 +13784,7 @@
         <v>711</v>
       </c>
       <c r="F146" s="17" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="G146" s="1" t="s">
         <v>711</v>
@@ -13839,7 +13826,7 @@
         <v>394</v>
       </c>
       <c r="B147" s="32" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>711</v>
@@ -13851,7 +13838,7 @@
         <v>711</v>
       </c>
       <c r="F147" s="17" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="G147" s="1" t="s">
         <v>711</v>
@@ -13894,7 +13881,7 @@
         <v>395</v>
       </c>
       <c r="B148" s="32" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>711</v>
@@ -13906,7 +13893,7 @@
         <v>711</v>
       </c>
       <c r="F148" s="17" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="G148" s="1" t="s">
         <v>711</v>
@@ -13948,7 +13935,7 @@
         <v>397</v>
       </c>
       <c r="B149" s="32" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>711</v>
@@ -13960,7 +13947,7 @@
         <v>711</v>
       </c>
       <c r="F149" s="17" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="G149" s="1" t="s">
         <v>711</v>
@@ -14002,7 +13989,7 @@
         <v>399</v>
       </c>
       <c r="B150" s="32" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>711</v>
@@ -14014,7 +14001,7 @@
         <v>711</v>
       </c>
       <c r="F150" s="17" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="G150" s="1" t="s">
         <v>711</v>
@@ -14059,7 +14046,7 @@
         <v>8</v>
       </c>
       <c r="B151" s="32" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>711</v>
@@ -14113,7 +14100,7 @@
         <v>404</v>
       </c>
       <c r="B152" s="32" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>711</v>
@@ -14125,7 +14112,7 @@
         <v>711</v>
       </c>
       <c r="F152" s="17" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="G152" s="1" t="s">
         <v>711</v>
@@ -14168,7 +14155,7 @@
         <v>406</v>
       </c>
       <c r="B153" s="32" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>711</v>
@@ -14180,7 +14167,7 @@
         <v>711</v>
       </c>
       <c r="F153" s="17" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G153" s="1" t="s">
         <v>711</v>
@@ -14222,7 +14209,7 @@
         <v>408</v>
       </c>
       <c r="B154" s="32" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>711</v>
@@ -14234,7 +14221,7 @@
         <v>711</v>
       </c>
       <c r="F154" s="17" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="G154" s="1" t="s">
         <v>711</v>
@@ -14276,7 +14263,7 @@
         <v>411</v>
       </c>
       <c r="B155" s="32" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>711</v>
@@ -14288,7 +14275,7 @@
         <v>711</v>
       </c>
       <c r="F155" s="17" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="G155" s="1" t="s">
         <v>711</v>
@@ -14330,7 +14317,7 @@
         <v>413</v>
       </c>
       <c r="B156" s="32" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>711</v>
@@ -14342,7 +14329,7 @@
         <v>711</v>
       </c>
       <c r="F156" s="17" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="G156" s="1" t="s">
         <v>711</v>
@@ -14384,7 +14371,7 @@
         <v>416</v>
       </c>
       <c r="B157" s="32" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>711</v>
@@ -14396,7 +14383,7 @@
         <v>711</v>
       </c>
       <c r="F157" s="17" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="G157" s="1" t="s">
         <v>711</v>
@@ -14439,7 +14426,7 @@
         <v>417</v>
       </c>
       <c r="B158" s="32" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>711</v>
@@ -14451,7 +14438,7 @@
         <v>711</v>
       </c>
       <c r="F158" s="17" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="G158" s="1" t="s">
         <v>711</v>
@@ -14493,7 +14480,7 @@
         <v>419</v>
       </c>
       <c r="B159" s="32" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>711</v>
@@ -14547,7 +14534,7 @@
         <v>421</v>
       </c>
       <c r="B160" s="32" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>711</v>
@@ -14559,7 +14546,7 @@
         <v>711</v>
       </c>
       <c r="F160" s="17" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="G160" s="1" t="s">
         <v>711</v>
@@ -14601,7 +14588,7 @@
         <v>423</v>
       </c>
       <c r="B161" s="32" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>711</v>
@@ -14655,7 +14642,7 @@
         <v>425</v>
       </c>
       <c r="B162" s="32" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>711</v>
@@ -14667,7 +14654,7 @@
         <v>711</v>
       </c>
       <c r="F162" s="17" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="G162" s="1" t="s">
         <v>711</v>
@@ -14712,7 +14699,7 @@
         <v>427</v>
       </c>
       <c r="B163" s="32" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>711</v>
@@ -14724,7 +14711,7 @@
         <v>711</v>
       </c>
       <c r="F163" s="17" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="G163" s="1" t="s">
         <v>711</v>
@@ -14766,7 +14753,7 @@
         <v>429</v>
       </c>
       <c r="B164" s="32" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>711</v>
@@ -14778,7 +14765,7 @@
         <v>711</v>
       </c>
       <c r="F164" s="17" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="G164" s="1" t="s">
         <v>711</v>
@@ -14820,7 +14807,7 @@
         <v>432</v>
       </c>
       <c r="B165" s="32" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>711</v>
@@ -14832,7 +14819,7 @@
         <v>711</v>
       </c>
       <c r="F165" s="17" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="G165" s="1" t="s">
         <v>711</v>
@@ -14874,7 +14861,7 @@
         <v>434</v>
       </c>
       <c r="B166" s="32" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>711</v>
@@ -14886,7 +14873,7 @@
         <v>711</v>
       </c>
       <c r="F166" s="17" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="G166" s="1" t="s">
         <v>711</v>
@@ -14929,7 +14916,7 @@
         <v>435</v>
       </c>
       <c r="B167" s="32" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>711</v>
@@ -14941,7 +14928,7 @@
         <v>711</v>
       </c>
       <c r="F167" s="17" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="G167" s="1" t="s">
         <v>711</v>
@@ -14986,7 +14973,7 @@
         <v>437</v>
       </c>
       <c r="B168" s="32" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>711</v>
@@ -14998,7 +14985,7 @@
         <v>711</v>
       </c>
       <c r="F168" s="17" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="G168" s="1" t="s">
         <v>711</v>
@@ -15040,7 +15027,7 @@
         <v>440</v>
       </c>
       <c r="B169" s="32" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>711</v>
@@ -15052,7 +15039,7 @@
         <v>711</v>
       </c>
       <c r="F169" s="17" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="G169" s="1" t="s">
         <v>711</v>
@@ -15097,7 +15084,7 @@
         <v>442</v>
       </c>
       <c r="B170" s="32" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>711</v>
@@ -15109,7 +15096,7 @@
         <v>711</v>
       </c>
       <c r="F170" s="17" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="G170" s="1" t="s">
         <v>711</v>
@@ -15151,7 +15138,7 @@
         <v>444</v>
       </c>
       <c r="B171" s="32" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>711</v>
@@ -15163,7 +15150,7 @@
         <v>711</v>
       </c>
       <c r="F171" s="17" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="G171" s="1" t="s">
         <v>711</v>
@@ -15208,7 +15195,7 @@
         <v>180</v>
       </c>
       <c r="B172" s="32" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>711</v>
@@ -15220,7 +15207,7 @@
         <v>711</v>
       </c>
       <c r="F172" s="17" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="G172" s="1" t="s">
         <v>711</v>
@@ -15263,7 +15250,7 @@
         <v>446</v>
       </c>
       <c r="B173" s="32" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>711</v>
@@ -15275,7 +15262,7 @@
         <v>711</v>
       </c>
       <c r="F173" s="17" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="G173" s="1" t="s">
         <v>711</v>
@@ -15317,7 +15304,7 @@
         <v>177</v>
       </c>
       <c r="B174" s="32" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>711</v>
@@ -15329,7 +15316,7 @@
         <v>711</v>
       </c>
       <c r="F174" s="17" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="G174" s="1" t="s">
         <v>711</v>
@@ -15372,7 +15359,7 @@
         <v>449</v>
       </c>
       <c r="B175" s="32" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>711</v>
@@ -15384,7 +15371,7 @@
         <v>711</v>
       </c>
       <c r="F175" s="17" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="G175" s="1" t="s">
         <v>711</v>
@@ -15426,7 +15413,7 @@
         <v>451</v>
       </c>
       <c r="B176" s="32" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>711</v>
@@ -15438,7 +15425,7 @@
         <v>711</v>
       </c>
       <c r="F176" s="17" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="G176" s="1" t="s">
         <v>711</v>
@@ -15480,7 +15467,7 @@
         <v>453</v>
       </c>
       <c r="B177" s="32" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>711</v>
@@ -15492,7 +15479,7 @@
         <v>711</v>
       </c>
       <c r="F177" s="17" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="G177" s="1" t="s">
         <v>711</v>
@@ -15534,7 +15521,7 @@
         <v>455</v>
       </c>
       <c r="B178" s="32" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>711</v>
@@ -15546,7 +15533,7 @@
         <v>711</v>
       </c>
       <c r="F178" s="17" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="G178" s="1" t="s">
         <v>711</v>
@@ -15586,7 +15573,7 @@
         <v>457</v>
       </c>
       <c r="B179" s="32" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>711</v>
@@ -15598,7 +15585,7 @@
         <v>711</v>
       </c>
       <c r="F179" s="17" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="G179" s="1" t="s">
         <v>711</v>
@@ -15640,7 +15627,7 @@
         <v>460</v>
       </c>
       <c r="B180" s="32" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>711</v>
@@ -15652,7 +15639,7 @@
         <v>711</v>
       </c>
       <c r="F180" s="17" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="G180" s="1" t="s">
         <v>711</v>
@@ -15697,7 +15684,7 @@
         <v>463</v>
       </c>
       <c r="B181" s="32" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>711</v>
@@ -15709,7 +15696,7 @@
         <v>711</v>
       </c>
       <c r="F181" s="17" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="G181" s="1" t="s">
         <v>711</v>
@@ -15754,7 +15741,7 @@
         <v>465</v>
       </c>
       <c r="B182" s="32" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>711</v>
@@ -15811,7 +15798,7 @@
         <v>467</v>
       </c>
       <c r="B183" s="32" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>711</v>
@@ -15823,7 +15810,7 @@
         <v>711</v>
       </c>
       <c r="F183" s="17" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="G183" s="1" t="s">
         <v>711</v>
@@ -15865,7 +15852,7 @@
         <v>470</v>
       </c>
       <c r="B184" s="32" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>711</v>
@@ -15877,7 +15864,7 @@
         <v>711</v>
       </c>
       <c r="F184" s="17" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="G184" s="1" t="s">
         <v>711</v>
@@ -15919,7 +15906,7 @@
         <v>472</v>
       </c>
       <c r="B185" s="32" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>711</v>
@@ -15931,7 +15918,7 @@
         <v>711</v>
       </c>
       <c r="F185" s="17" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="G185" s="1" t="s">
         <v>711</v>
@@ -15971,7 +15958,7 @@
         <v>473</v>
       </c>
       <c r="B186" s="32" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>711</v>
@@ -15983,7 +15970,7 @@
         <v>711</v>
       </c>
       <c r="F186" s="17" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="G186" s="1" t="s">
         <v>711</v>
@@ -16025,7 +16012,7 @@
         <v>475</v>
       </c>
       <c r="B187" s="32" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>711</v>
@@ -16037,7 +16024,7 @@
         <v>711</v>
       </c>
       <c r="F187" s="17" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="G187" s="1" t="s">
         <v>711</v>
@@ -16082,7 +16069,7 @@
         <v>477</v>
       </c>
       <c r="B188" s="32" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>711</v>
@@ -16094,7 +16081,7 @@
         <v>711</v>
       </c>
       <c r="F188" s="17" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="G188" s="1" t="s">
         <v>711</v>
@@ -16136,7 +16123,7 @@
         <v>480</v>
       </c>
       <c r="B189" s="32" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>711</v>
@@ -16148,7 +16135,7 @@
         <v>711</v>
       </c>
       <c r="F189" s="17" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="G189" s="1" t="s">
         <v>711</v>
@@ -16190,7 +16177,7 @@
         <v>482</v>
       </c>
       <c r="B190" s="32" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>711</v>
@@ -16202,7 +16189,7 @@
         <v>711</v>
       </c>
       <c r="F190" s="17" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="G190" s="1" t="s">
         <v>711</v>
@@ -16244,7 +16231,7 @@
         <v>485</v>
       </c>
       <c r="B191" s="32" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>711</v>
@@ -16256,7 +16243,7 @@
         <v>711</v>
       </c>
       <c r="F191" s="17" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="G191" s="1" t="s">
         <v>711</v>
@@ -16301,7 +16288,7 @@
         <v>487</v>
       </c>
       <c r="B192" s="32" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>711</v>
@@ -16313,7 +16300,7 @@
         <v>711</v>
       </c>
       <c r="F192" s="17" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="G192" s="1" t="s">
         <v>711</v>
@@ -16355,7 +16342,7 @@
         <v>490</v>
       </c>
       <c r="B193" s="32" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>711</v>
@@ -16367,7 +16354,7 @@
         <v>711</v>
       </c>
       <c r="F193" s="17" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="G193" s="1" t="s">
         <v>711</v>
@@ -16409,7 +16396,7 @@
         <v>492</v>
       </c>
       <c r="B194" s="32" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>711</v>
@@ -16421,7 +16408,7 @@
         <v>711</v>
       </c>
       <c r="F194" s="17" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="G194" s="1" t="s">
         <v>711</v>
@@ -16463,7 +16450,7 @@
         <v>494</v>
       </c>
       <c r="B195" s="32" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>711</v>
@@ -16475,7 +16462,7 @@
         <v>711</v>
       </c>
       <c r="F195" s="17" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="G195" s="1" t="s">
         <v>711</v>
@@ -16517,7 +16504,7 @@
         <v>496</v>
       </c>
       <c r="B196" s="32" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>711</v>
@@ -16529,7 +16516,7 @@
         <v>711</v>
       </c>
       <c r="F196" s="17" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="G196" s="1" t="s">
         <v>711</v>
@@ -16571,7 +16558,7 @@
         <v>498</v>
       </c>
       <c r="B197" s="32" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>711</v>
@@ -16623,7 +16610,7 @@
         <v>501</v>
       </c>
       <c r="B198" s="32" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>711</v>
@@ -16635,7 +16622,7 @@
         <v>711</v>
       </c>
       <c r="F198" s="17" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="G198" s="1" t="s">
         <v>711</v>
@@ -16677,7 +16664,7 @@
         <v>503</v>
       </c>
       <c r="B199" s="32" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>711</v>
@@ -16689,7 +16676,7 @@
         <v>711</v>
       </c>
       <c r="F199" s="17" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="G199" s="1" t="s">
         <v>711</v>
@@ -16731,7 +16718,7 @@
         <v>506</v>
       </c>
       <c r="B200" s="32" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>711</v>
@@ -16743,7 +16730,7 @@
         <v>711</v>
       </c>
       <c r="F200" s="17" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="G200" s="1" t="s">
         <v>711</v>
@@ -16788,7 +16775,7 @@
         <v>508</v>
       </c>
       <c r="B201" s="32" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>711</v>
@@ -16800,7 +16787,7 @@
         <v>711</v>
       </c>
       <c r="F201" s="17" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="G201" s="1" t="s">
         <v>711</v>
@@ -16842,7 +16829,7 @@
         <v>510</v>
       </c>
       <c r="B202" s="32" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>711</v>
@@ -16854,7 +16841,7 @@
         <v>711</v>
       </c>
       <c r="F202" s="17" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="G202" s="1" t="s">
         <v>711</v>
@@ -16899,7 +16886,7 @@
         <v>512</v>
       </c>
       <c r="B203" s="32" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>711</v>
@@ -16911,7 +16898,7 @@
         <v>711</v>
       </c>
       <c r="F203" s="17" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="G203" s="1" t="s">
         <v>711</v>
@@ -16954,7 +16941,7 @@
         <v>513</v>
       </c>
       <c r="B204" s="32" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>711</v>
@@ -16966,7 +16953,7 @@
         <v>711</v>
       </c>
       <c r="F204" s="17" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="G204" s="1" t="s">
         <v>711</v>
@@ -17008,7 +16995,7 @@
         <v>515</v>
       </c>
       <c r="B205" s="32" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>711</v>
@@ -17020,7 +17007,7 @@
         <v>711</v>
       </c>
       <c r="F205" s="17" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="G205" s="1" t="s">
         <v>711</v>
@@ -17065,7 +17052,7 @@
         <v>39</v>
       </c>
       <c r="B206" s="32" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>711</v>
@@ -17077,7 +17064,7 @@
         <v>711</v>
       </c>
       <c r="F206" s="17" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="G206" s="1" t="s">
         <v>711</v>
@@ -17120,7 +17107,7 @@
         <v>517</v>
       </c>
       <c r="B207" s="32" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>711</v>
@@ -17132,7 +17119,7 @@
         <v>711</v>
       </c>
       <c r="F207" s="17" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="G207" s="1" t="s">
         <v>711</v>
@@ -17174,7 +17161,7 @@
         <v>519</v>
       </c>
       <c r="B208" s="32" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>711</v>
@@ -17228,7 +17215,7 @@
         <v>522</v>
       </c>
       <c r="B209" s="32" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>711</v>
@@ -17285,7 +17272,7 @@
         <v>92</v>
       </c>
       <c r="B210" s="32" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>711</v>
@@ -17297,7 +17284,7 @@
         <v>711</v>
       </c>
       <c r="F210" s="17" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="G210" s="1" t="s">
         <v>711</v>
@@ -17339,7 +17326,7 @@
         <v>526</v>
       </c>
       <c r="B211" s="32" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>711</v>
@@ -17351,7 +17338,7 @@
         <v>711</v>
       </c>
       <c r="F211" s="17" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="G211" s="1" t="s">
         <v>711</v>
@@ -17396,7 +17383,7 @@
         <v>528</v>
       </c>
       <c r="B212" s="32" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>711</v>
@@ -17408,7 +17395,7 @@
         <v>711</v>
       </c>
       <c r="F212" s="17" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="G212" s="1" t="s">
         <v>711</v>
@@ -17450,7 +17437,7 @@
         <v>662</v>
       </c>
       <c r="B213" s="32" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>711</v>
@@ -17462,7 +17449,7 @@
         <v>711</v>
       </c>
       <c r="F213" s="17" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="G213" s="1" t="s">
         <v>711</v>
@@ -17507,7 +17494,7 @@
         <v>531</v>
       </c>
       <c r="B214" s="32" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>711</v>
@@ -17519,7 +17506,7 @@
         <v>711</v>
       </c>
       <c r="F214" s="17" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="G214" s="1" t="s">
         <v>711</v>
@@ -17564,7 +17551,7 @@
         <v>533</v>
       </c>
       <c r="B215" s="32" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>711</v>
@@ -17576,7 +17563,7 @@
         <v>711</v>
       </c>
       <c r="F215" s="17" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="G215" s="1" t="s">
         <v>711</v>
@@ -17618,7 +17605,7 @@
         <v>535</v>
       </c>
       <c r="B216" s="32" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>711</v>
@@ -17630,7 +17617,7 @@
         <v>711</v>
       </c>
       <c r="F216" s="17" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="G216" s="1" t="s">
         <v>711</v>
@@ -17672,7 +17659,7 @@
         <v>537</v>
       </c>
       <c r="B217" s="32" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>711</v>
@@ -17684,7 +17671,7 @@
         <v>711</v>
       </c>
       <c r="F217" s="17" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="G217" s="1" t="s">
         <v>711</v>
@@ -17726,7 +17713,7 @@
         <v>539</v>
       </c>
       <c r="B218" s="32" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>711</v>
@@ -17738,7 +17725,7 @@
         <v>711</v>
       </c>
       <c r="F218" s="17" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="G218" s="1" t="s">
         <v>711</v>
@@ -17783,7 +17770,7 @@
         <v>541</v>
       </c>
       <c r="B219" s="32" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>711</v>
@@ -17795,7 +17782,7 @@
         <v>711</v>
       </c>
       <c r="F219" s="17" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="G219" s="1" t="s">
         <v>711</v>
@@ -17837,7 +17824,7 @@
         <v>544</v>
       </c>
       <c r="B220" s="32" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>711</v>
@@ -17849,7 +17836,7 @@
         <v>711</v>
       </c>
       <c r="F220" s="17" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="G220" s="1" t="s">
         <v>711</v>
@@ -17894,7 +17881,7 @@
         <v>546</v>
       </c>
       <c r="B221" s="32" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>711</v>
@@ -17906,7 +17893,7 @@
         <v>711</v>
       </c>
       <c r="F221" s="17" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="G221" s="1" t="s">
         <v>711</v>
@@ -17951,7 +17938,7 @@
         <v>88</v>
       </c>
       <c r="B222" s="32" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>711</v>
@@ -17963,7 +17950,7 @@
         <v>711</v>
       </c>
       <c r="F222" s="17" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="G222" s="1" t="s">
         <v>711</v>
@@ -18008,7 +17995,7 @@
         <v>549</v>
       </c>
       <c r="B223" s="32" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>711</v>
@@ -18062,7 +18049,7 @@
         <v>551</v>
       </c>
       <c r="B224" s="32" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>711</v>
@@ -18074,7 +18061,7 @@
         <v>711</v>
       </c>
       <c r="F224" s="17" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="G224" s="1" t="s">
         <v>711</v>
@@ -18117,7 +18104,7 @@
         <v>552</v>
       </c>
       <c r="B225" s="32" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>711</v>
@@ -18129,7 +18116,7 @@
         <v>711</v>
       </c>
       <c r="F225" s="17" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="G225" s="1" t="s">
         <v>711</v>
@@ -18171,7 +18158,7 @@
         <v>554</v>
       </c>
       <c r="B226" s="32" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>711</v>
@@ -18183,7 +18170,7 @@
         <v>711</v>
       </c>
       <c r="F226" s="17" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="G226" s="1" t="s">
         <v>711</v>
@@ -18228,7 +18215,7 @@
         <v>366</v>
       </c>
       <c r="B227" s="32" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>711</v>
@@ -18240,7 +18227,7 @@
         <v>711</v>
       </c>
       <c r="F227" s="17" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="G227" s="1" t="s">
         <v>711</v>
@@ -18285,7 +18272,7 @@
         <v>557</v>
       </c>
       <c r="B228" s="32" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>711</v>
@@ -18297,7 +18284,7 @@
         <v>711</v>
       </c>
       <c r="F228" s="17" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="G228" s="1" t="s">
         <v>711</v>
@@ -18342,7 +18329,7 @@
         <v>559</v>
       </c>
       <c r="B229" s="32" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>711</v>
@@ -18354,7 +18341,7 @@
         <v>711</v>
       </c>
       <c r="F229" s="17" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="G229" s="1" t="s">
         <v>711</v>
@@ -18396,7 +18383,7 @@
         <v>561</v>
       </c>
       <c r="B230" s="32" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>711</v>
@@ -18451,7 +18438,7 @@
         <v>563</v>
       </c>
       <c r="B231" s="32" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>711</v>
@@ -18463,7 +18450,7 @@
         <v>711</v>
       </c>
       <c r="F231" s="17" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="G231" s="1" t="s">
         <v>711</v>
@@ -18506,7 +18493,7 @@
         <v>564</v>
       </c>
       <c r="B232" s="32" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>711</v>
@@ -18518,7 +18505,7 @@
         <v>711</v>
       </c>
       <c r="F232" s="17" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="G232" s="1" t="s">
         <v>711</v>
@@ -18560,7 +18547,7 @@
         <v>566</v>
       </c>
       <c r="B233" s="32" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>711</v>
@@ -18572,7 +18559,7 @@
         <v>711</v>
       </c>
       <c r="F233" s="17" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="G233" s="1" t="s">
         <v>711</v>
@@ -18615,7 +18602,7 @@
         <v>568</v>
       </c>
       <c r="B234" s="32" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>711</v>
@@ -18627,7 +18614,7 @@
         <v>711</v>
       </c>
       <c r="F234" s="17" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="G234" s="1" t="s">
         <v>711</v>
@@ -18672,7 +18659,7 @@
         <v>570</v>
       </c>
       <c r="B235" s="32" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>711</v>
@@ -18684,7 +18671,7 @@
         <v>711</v>
       </c>
       <c r="F235" s="17" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="G235" s="1" t="s">
         <v>711</v>
@@ -18727,7 +18714,7 @@
         <v>572</v>
       </c>
       <c r="B236" s="32" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>711</v>
@@ -18739,7 +18726,7 @@
         <v>711</v>
       </c>
       <c r="F236" s="17" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="G236" s="1" t="s">
         <v>711</v>
@@ -18784,7 +18771,7 @@
         <v>575</v>
       </c>
       <c r="B237" s="32" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>711</v>
@@ -18796,7 +18783,7 @@
         <v>711</v>
       </c>
       <c r="F237" s="17" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="G237" s="1" t="s">
         <v>711</v>
@@ -18841,7 +18828,7 @@
         <v>577</v>
       </c>
       <c r="B238" s="32" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>711</v>
@@ -18853,7 +18840,7 @@
         <v>711</v>
       </c>
       <c r="F238" s="17" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="G238" s="1" t="s">
         <v>711</v>
@@ -18896,7 +18883,7 @@
         <v>578</v>
       </c>
       <c r="B239" s="32" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>711</v>
@@ -18908,7 +18895,7 @@
         <v>711</v>
       </c>
       <c r="F239" s="17" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="G239" s="1" t="s">
         <v>711</v>
@@ -18951,7 +18938,7 @@
         <v>579</v>
       </c>
       <c r="B240" s="32" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>711</v>
@@ -19005,7 +18992,7 @@
         <v>581</v>
       </c>
       <c r="B241" s="32" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>711</v>
@@ -19017,7 +19004,7 @@
         <v>711</v>
       </c>
       <c r="F241" s="17" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G241" s="1" t="s">
         <v>711</v>
@@ -19062,7 +19049,7 @@
         <v>583</v>
       </c>
       <c r="B242" s="32" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>711</v>
@@ -19074,7 +19061,7 @@
         <v>711</v>
       </c>
       <c r="F242" s="17" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="G242" s="1" t="s">
         <v>711</v>
@@ -19116,7 +19103,7 @@
         <v>586</v>
       </c>
       <c r="B243" s="32" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>711</v>
@@ -19128,7 +19115,7 @@
         <v>711</v>
       </c>
       <c r="F243" s="17" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="G243" s="1" t="s">
         <v>711</v>
@@ -19170,7 +19157,7 @@
         <v>588</v>
       </c>
       <c r="B244" s="32" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>711</v>
@@ -19182,7 +19169,7 @@
         <v>711</v>
       </c>
       <c r="F244" s="17" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="G244" s="1" t="s">
         <v>711</v>
@@ -19227,7 +19214,7 @@
         <v>590</v>
       </c>
       <c r="B245" s="32" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>711</v>
@@ -19239,7 +19226,7 @@
         <v>711</v>
       </c>
       <c r="F245" s="17" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="G245" s="1" t="s">
         <v>711</v>
@@ -19281,7 +19268,7 @@
         <v>593</v>
       </c>
       <c r="B246" s="32" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>711</v>
@@ -19293,7 +19280,7 @@
         <v>711</v>
       </c>
       <c r="F246" s="17" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="G246" s="1" t="s">
         <v>711</v>
@@ -19333,7 +19320,7 @@
         <v>595</v>
       </c>
       <c r="B247" s="32" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>711</v>
@@ -19345,7 +19332,7 @@
         <v>711</v>
       </c>
       <c r="F247" s="17" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="G247" s="1" t="s">
         <v>711</v>
@@ -19387,7 +19374,7 @@
         <v>597</v>
       </c>
       <c r="B248" s="32" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>711</v>
@@ -19399,7 +19386,7 @@
         <v>711</v>
       </c>
       <c r="F248" s="17" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="G248" s="1" t="s">
         <v>711</v>
@@ -19441,7 +19428,7 @@
         <v>599</v>
       </c>
       <c r="B249" s="32" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>711</v>
@@ -19453,7 +19440,7 @@
         <v>711</v>
       </c>
       <c r="F249" s="17" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="G249" s="1" t="s">
         <v>711</v>
@@ -19495,7 +19482,7 @@
         <v>601</v>
       </c>
       <c r="B250" s="32" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>711</v>
@@ -19507,7 +19494,7 @@
         <v>711</v>
       </c>
       <c r="F250" s="17" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="G250" s="1" t="s">
         <v>711</v>
@@ -19552,7 +19539,7 @@
         <v>603</v>
       </c>
       <c r="B251" s="32" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>711</v>
@@ -19564,7 +19551,7 @@
         <v>711</v>
       </c>
       <c r="F251" s="17" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G251" s="1" t="s">
         <v>711</v>
@@ -19606,7 +19593,7 @@
         <v>605</v>
       </c>
       <c r="B252" s="32" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>711</v>
@@ -19663,7 +19650,7 @@
         <v>607</v>
       </c>
       <c r="B253" s="32" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>711</v>
@@ -19675,7 +19662,7 @@
         <v>711</v>
       </c>
       <c r="F253" s="17" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="G253" s="1" t="s">
         <v>711</v>
@@ -19715,7 +19702,7 @@
         <v>608</v>
       </c>
       <c r="B254" s="32" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>711</v>
@@ -19727,7 +19714,7 @@
         <v>711</v>
       </c>
       <c r="F254" s="17" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="G254" s="1" t="s">
         <v>711</v>
@@ -19772,7 +19759,7 @@
         <v>610</v>
       </c>
       <c r="B255" s="32" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>711</v>
@@ -19826,7 +19813,7 @@
         <v>612</v>
       </c>
       <c r="B256" s="32" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>711</v>
@@ -19838,7 +19825,7 @@
         <v>711</v>
       </c>
       <c r="F256" s="17" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="G256" s="1" t="s">
         <v>711</v>
@@ -19883,7 +19870,7 @@
         <v>614</v>
       </c>
       <c r="B257" s="32" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>711</v>
@@ -19895,7 +19882,7 @@
         <v>711</v>
       </c>
       <c r="F257" s="17" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="G257" s="1" t="s">
         <v>711</v>
@@ -19937,7 +19924,7 @@
         <v>618</v>
       </c>
       <c r="B258" s="32" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>711</v>
@@ -19949,7 +19936,7 @@
         <v>711</v>
       </c>
       <c r="F258" s="17" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="G258" s="1" t="s">
         <v>711</v>
@@ -19991,7 +19978,7 @@
         <v>620</v>
       </c>
       <c r="B259" s="32" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>711</v>
@@ -20045,7 +20032,7 @@
         <v>622</v>
       </c>
       <c r="B260" s="32" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>711</v>
@@ -20102,7 +20089,7 @@
         <v>624</v>
       </c>
       <c r="B261" s="32" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>711</v>
@@ -20114,7 +20101,7 @@
         <v>711</v>
       </c>
       <c r="F261" s="17" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="G261" s="1" t="s">
         <v>711</v>
@@ -20156,7 +20143,7 @@
         <v>626</v>
       </c>
       <c r="B262" s="32" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>711</v>
@@ -20168,7 +20155,7 @@
         <v>711</v>
       </c>
       <c r="F262" s="17" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="G262" s="1" t="s">
         <v>711</v>
@@ -20211,7 +20198,7 @@
         <v>627</v>
       </c>
       <c r="B263" s="32" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>711</v>
@@ -20223,7 +20210,7 @@
         <v>711</v>
       </c>
       <c r="F263" s="17" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="G263" s="1" t="s">
         <v>711</v>
@@ -20265,7 +20252,7 @@
         <v>629</v>
       </c>
       <c r="B264" s="32" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="C264" s="1" t="s">
         <v>711</v>
@@ -20277,7 +20264,7 @@
         <v>711</v>
       </c>
       <c r="F264" s="17" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="G264" s="1" t="s">
         <v>711</v>
@@ -20320,7 +20307,7 @@
         <v>630</v>
       </c>
       <c r="B265" s="32" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>711</v>
@@ -20332,7 +20319,7 @@
         <v>711</v>
       </c>
       <c r="F265" s="17" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="G265" s="1" t="s">
         <v>711</v>
@@ -20377,7 +20364,7 @@
         <v>632</v>
       </c>
       <c r="B266" s="32" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>711</v>
@@ -20389,7 +20376,7 @@
         <v>711</v>
       </c>
       <c r="F266" s="17" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="G266" s="1" t="s">
         <v>711</v>
@@ -20431,7 +20418,7 @@
         <v>634</v>
       </c>
       <c r="B267" s="32" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>711</v>
@@ -20443,7 +20430,7 @@
         <v>711</v>
       </c>
       <c r="F267" s="17" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="G267" s="1" t="s">
         <v>711</v>
@@ -20488,7 +20475,7 @@
         <v>636</v>
       </c>
       <c r="B268" s="32" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>711</v>
@@ -20500,7 +20487,7 @@
         <v>711</v>
       </c>
       <c r="F268" s="17" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="G268" s="1" t="s">
         <v>711</v>
@@ -20542,7 +20529,7 @@
         <v>638</v>
       </c>
       <c r="B269" s="32" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>711</v>
@@ -20554,7 +20541,7 @@
         <v>711</v>
       </c>
       <c r="F269" s="17" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="G269" s="1" t="s">
         <v>711</v>
@@ -20597,7 +20584,7 @@
         <v>639</v>
       </c>
       <c r="B270" s="32" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>711</v>
@@ -20609,7 +20596,7 @@
         <v>711</v>
       </c>
       <c r="F270" s="17" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="G270" s="1" t="s">
         <v>711</v>
@@ -20654,7 +20641,7 @@
         <v>641</v>
       </c>
       <c r="B271" s="32" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="C271" s="1" t="s">
         <v>711</v>
@@ -20666,7 +20653,7 @@
         <v>711</v>
       </c>
       <c r="F271" s="17" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="G271" s="1" t="s">
         <v>711</v>
@@ -20708,7 +20695,7 @@
         <v>181</v>
       </c>
       <c r="B272" s="32" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="C272" s="1" t="s">
         <v>711</v>
@@ -20720,7 +20707,7 @@
         <v>711</v>
       </c>
       <c r="F272" s="17" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="G272" s="1" t="s">
         <v>711</v>
@@ -20762,7 +20749,7 @@
         <v>231</v>
       </c>
       <c r="B273" s="32" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>711</v>
@@ -20774,7 +20761,7 @@
         <v>711</v>
       </c>
       <c r="F273" s="17" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="G273" s="1" t="s">
         <v>711</v>
@@ -22601,13 +22588,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D338:E1048576 D1:E273">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="County">
+    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="County">
       <formula>NOT(ISERROR(SEARCH("County",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Town of">
+    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="Town of">
       <formula>NOT(ISERROR(SEARCH("Town of",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="City of">
+    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="City of">
       <formula>NOT(ISERROR(SEARCH("City of",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23549,7 +23536,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -23930,7 +23917,7 @@
         <v>764</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>765</v>
@@ -23947,7 +23934,7 @@
         <v>764</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D14" s="16" t="s">
         <v>765</v>
@@ -23992,7 +23979,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>764</v>
@@ -24009,7 +23996,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>776</v>

</xml_diff>

<commit_message>
Minor modifications to dataset and update README
</commit_message>
<xml_diff>
--- a/data/Colorado-Municipalities.xlsx
+++ b/data/Colorado-Municipalities.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="3" r:id="rId1"/>
@@ -6038,7 +6038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -27142,7 +27142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>